<commit_message>
Fix .gitignore to ignore exiobase
</commit_message>
<xml_diff>
--- a/config/sectors.xlsx
+++ b/config/sectors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A08603E-CAEC-48A4-AE6E-4C75249D5D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223B183C-2593-4E4B-B13C-094715AFB9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6932,7 +6932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C379D830-202D-4ECB-B7AD-7DF819B8A6BC}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>

</xml_diff>